<commit_message>
v2 + giffler escrito
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Documentos\IFNMG\TCC\Desenvolvimento_TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A10FBE3-6F19-44C0-9960-F0CEB6C8C54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646195F9-D891-4CE2-9FCF-BF5E1143EC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="309">
   <si>
     <t>BRKGA</t>
   </si>
@@ -960,7 +960,10 @@
     <t>v2 + gliffler</t>
   </si>
   <si>
-    <t>V2G % G</t>
+    <t>v2G ~ G</t>
+  </si>
+  <si>
+    <t>V2+G % G</t>
   </si>
 </sst>
 </file>
@@ -7899,8 +7902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595BCFD6-D5E4-4B60-8194-9ED1C2C22A4C}">
   <dimension ref="A1:AX78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN3" sqref="AN3"/>
+    <sheetView tabSelected="1" topLeftCell="E46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AJ79" sqref="AJ79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7908,19 +7911,24 @@
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="19" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" style="19" customWidth="1"/>
-    <col min="11" max="12" width="10.140625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" style="19" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="10.140625" style="19" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="9.28515625" style="19" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" style="19" customWidth="1"/>
-    <col min="20" max="21" width="9.140625" style="22"/>
+    <col min="16" max="16" width="9.28515625" style="19" customWidth="1"/>
+    <col min="17" max="18" width="9.28515625" style="19" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" style="19" hidden="1" customWidth="1"/>
+    <col min="20" max="21" width="0" style="22" hidden="1" customWidth="1"/>
+    <col min="22" max="23" width="0" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.28515625" style="19" customWidth="1"/>
-    <col min="28" max="28" width="10.28515625" style="19" customWidth="1"/>
-    <col min="29" max="32" width="9.140625" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" style="19" customWidth="1"/>
+    <col min="26" max="27" width="9.28515625" style="19" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="10.28515625" style="19" hidden="1" customWidth="1"/>
+    <col min="29" max="32" width="9.140625" hidden="1" customWidth="1"/>
     <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="34" max="36" width="9.28515625" style="19" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="10.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
@@ -8055,8 +8063,11 @@
       <c r="AK2" s="20" t="s">
         <v>160</v>
       </c>
+      <c r="AL2" s="20" t="s">
+        <v>307</v>
+      </c>
       <c r="AM2" s="20" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AN2" s="20" t="s">
         <v>155</v>
@@ -11464,6 +11475,27 @@
       <c r="AG28" s="24" t="s">
         <v>260</v>
       </c>
+      <c r="AH28" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="AI28" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="AJ28" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK28" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL28" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="AM28" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN28" s="20" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -14866,6 +14898,27 @@
       </c>
       <c r="AG54" s="24" t="s">
         <v>261</v>
+      </c>
+      <c r="AH54" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="AI54" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="AJ54" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK54" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="AL54" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="AM54" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="AN54" s="20" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:50" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lipeza de comentários e organização
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\OneDrive\Documentos\IFNMG\TCC\Desenvolvimento_TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E625AA21-1375-4B54-8564-E87D7AF10E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA8855B8-1734-40D1-9E1E-BA39DED704BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="2" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="3" r:id="rId2"/>
     <sheet name="Planilha2" sheetId="4" r:id="rId3"/>
-    <sheet name="Planilha4" sheetId="6" r:id="rId4"/>
-    <sheet name="Planilha3" sheetId="5" r:id="rId5"/>
-    <sheet name="Planilha5" sheetId="7" r:id="rId6"/>
+    <sheet name="Planilha3" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="317">
   <si>
     <t>BRKGA</t>
   </si>
@@ -975,6 +973,21 @@
   </si>
   <si>
     <t>V3 % G</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>diag</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>down</t>
+  </si>
+  <si>
+    <t>right</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1195,17 +1208,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7949,7 +7961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595BCFD6-D5E4-4B60-8194-9ED1C2C22A4C}">
   <dimension ref="A1:BN78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="AM37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AX30" sqref="AX30"/>
     </sheetView>
   </sheetViews>
@@ -7969,7 +7981,7 @@
     <col min="24" max="24" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="27" width="9.28515625" style="19" customWidth="1"/>
     <col min="28" max="28" width="10.28515625" style="34" customWidth="1"/>
-    <col min="29" max="29" width="10.28515625" style="37" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="10.28515625" style="34" hidden="1" customWidth="1"/>
     <col min="31" max="34" width="9.140625" customWidth="1"/>
     <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
@@ -8247,7 +8259,7 @@
       <c r="AB3" s="34">
         <v>30.507000000000001</v>
       </c>
-      <c r="AC3" s="37">
+      <c r="AC3">
         <v>30.507000000000001</v>
       </c>
       <c r="AD3" s="34">
@@ -8421,7 +8433,7 @@
       <c r="AB4" s="34">
         <v>14.769</v>
       </c>
-      <c r="AC4" s="37">
+      <c r="AC4">
         <v>14.769</v>
       </c>
       <c r="AD4" s="34">
@@ -8595,7 +8607,7 @@
       <c r="AB5" s="34">
         <v>39.978000000000002</v>
       </c>
-      <c r="AC5" s="37">
+      <c r="AC5">
         <v>39.978000000000002</v>
       </c>
       <c r="AD5" s="34">
@@ -8769,7 +8781,7 @@
       <c r="AB6" s="34">
         <v>46.005000000000003</v>
       </c>
-      <c r="AC6" s="37">
+      <c r="AC6">
         <v>46.005000000000003</v>
       </c>
       <c r="AD6" s="34">
@@ -8943,7 +8955,7 @@
       <c r="AB7" s="34">
         <v>105.44499999999999</v>
       </c>
-      <c r="AC7" s="37">
+      <c r="AC7">
         <v>105.44499999999999</v>
       </c>
       <c r="AD7" s="34">
@@ -9117,7 +9129,7 @@
       <c r="AB8" s="34">
         <v>65.088999999999999</v>
       </c>
-      <c r="AC8" s="37">
+      <c r="AC8">
         <v>65.088999999999999</v>
       </c>
       <c r="AD8" s="34">
@@ -9291,7 +9303,7 @@
       <c r="AB9" s="34">
         <v>19.646000000000001</v>
       </c>
-      <c r="AC9" s="37">
+      <c r="AC9">
         <v>19.646000000000001</v>
       </c>
       <c r="AD9" s="34">
@@ -9465,7 +9477,7 @@
       <c r="AB10" s="34">
         <v>15.696999999999999</v>
       </c>
-      <c r="AC10" s="37">
+      <c r="AC10">
         <v>15.696999999999999</v>
       </c>
       <c r="AD10" s="34">
@@ -9639,7 +9651,7 @@
       <c r="AB11" s="34">
         <v>3.512</v>
       </c>
-      <c r="AC11" s="37">
+      <c r="AC11">
         <v>3.512</v>
       </c>
       <c r="AD11" s="34">
@@ -9813,7 +9825,7 @@
       <c r="AB12" s="34">
         <v>36.395000000000003</v>
       </c>
-      <c r="AC12" s="37">
+      <c r="AC12">
         <v>36.395000000000003</v>
       </c>
       <c r="AD12" s="34">
@@ -9987,7 +9999,7 @@
       <c r="AB13" s="34">
         <v>48.936</v>
       </c>
-      <c r="AC13" s="37">
+      <c r="AC13">
         <v>48.936</v>
       </c>
       <c r="AD13" s="34">
@@ -10161,7 +10173,7 @@
       <c r="AB14" s="34">
         <v>74.769000000000005</v>
       </c>
-      <c r="AC14" s="37">
+      <c r="AC14">
         <v>74.769000000000005</v>
       </c>
       <c r="AD14" s="34">
@@ -10335,7 +10347,7 @@
       <c r="AB15" s="34">
         <v>40.006</v>
       </c>
-      <c r="AC15" s="37">
+      <c r="AC15">
         <v>40.006</v>
       </c>
       <c r="AD15" s="34">
@@ -10509,7 +10521,7 @@
       <c r="AB16" s="34">
         <v>52.398000000000003</v>
       </c>
-      <c r="AC16" s="37">
+      <c r="AC16">
         <v>52.398000000000003</v>
       </c>
       <c r="AD16" s="34">
@@ -10683,7 +10695,7 @@
       <c r="AB17" s="34">
         <v>44.927</v>
       </c>
-      <c r="AC17" s="37">
+      <c r="AC17">
         <v>44.927</v>
       </c>
       <c r="AD17" s="34">
@@ -10857,7 +10869,7 @@
       <c r="AB18" s="34">
         <v>550.024</v>
       </c>
-      <c r="AC18" s="37">
+      <c r="AC18">
         <v>550.024</v>
       </c>
       <c r="AD18" s="34">
@@ -11031,7 +11043,7 @@
       <c r="AB19" s="34">
         <v>44.351999999999997</v>
       </c>
-      <c r="AC19" s="37">
+      <c r="AC19">
         <v>44.351999999999997</v>
       </c>
       <c r="AD19" s="34">
@@ -11205,7 +11217,7 @@
       <c r="AB20" s="34">
         <v>43.865000000000002</v>
       </c>
-      <c r="AC20" s="37">
+      <c r="AC20">
         <v>43.865000000000002</v>
       </c>
       <c r="AD20" s="34">
@@ -11379,7 +11391,7 @@
       <c r="AB21" s="34">
         <v>24.873999999999999</v>
       </c>
-      <c r="AC21" s="37">
+      <c r="AC21">
         <v>24.873999999999999</v>
       </c>
       <c r="AD21" s="34">
@@ -11553,7 +11565,7 @@
       <c r="AB22" s="34">
         <v>13.076000000000001</v>
       </c>
-      <c r="AC22" s="37">
+      <c r="AC22">
         <v>13.076000000000001</v>
       </c>
       <c r="AD22" s="34">
@@ -11727,7 +11739,7 @@
       <c r="AB23" s="34">
         <v>25.111000000000001</v>
       </c>
-      <c r="AC23" s="37">
+      <c r="AC23">
         <v>25.111000000000001</v>
       </c>
       <c r="AD23" s="34">
@@ -11901,7 +11913,7 @@
       <c r="AB24" s="34">
         <v>24.867000000000001</v>
       </c>
-      <c r="AC24" s="37">
+      <c r="AC24">
         <v>24.867000000000001</v>
       </c>
       <c r="AD24" s="34">
@@ -12075,7 +12087,7 @@
       <c r="AB25" s="34">
         <v>81.748999999999995</v>
       </c>
-      <c r="AC25" s="37">
+      <c r="AC25">
         <v>81.748999999999995</v>
       </c>
       <c r="AD25" s="34">
@@ -12249,7 +12261,7 @@
       <c r="AB26" s="34">
         <v>4.3559999999999999</v>
       </c>
-      <c r="AC26" s="37">
+      <c r="AC26">
         <v>4.3559999999999999</v>
       </c>
       <c r="AD26" s="34">
@@ -12413,7 +12425,7 @@
       <c r="AB28" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="AC28" s="38"/>
+      <c r="AC28" s="37"/>
       <c r="AD28" s="33" t="s">
         <v>160</v>
       </c>
@@ -12561,7 +12573,7 @@
       <c r="AB29" s="34">
         <v>3.3130000000000002</v>
       </c>
-      <c r="AC29" s="37">
+      <c r="AC29">
         <v>3.3130000000000002</v>
       </c>
       <c r="AD29" s="34">
@@ -12733,7 +12745,7 @@
       <c r="AB30" s="34">
         <v>30.239000000000001</v>
       </c>
-      <c r="AC30" s="37">
+      <c r="AC30">
         <v>30.239000000000001</v>
       </c>
       <c r="AD30" s="34">
@@ -12905,7 +12917,7 @@
       <c r="AB31" s="34">
         <v>49.323999999999998</v>
       </c>
-      <c r="AC31" s="37">
+      <c r="AC31">
         <v>49.323999999999998</v>
       </c>
       <c r="AD31" s="34">
@@ -13077,7 +13089,7 @@
       <c r="AB32" s="34">
         <v>4.0839999999999996</v>
       </c>
-      <c r="AC32" s="37">
+      <c r="AC32">
         <v>4.0839999999999996</v>
       </c>
       <c r="AD32" s="34">
@@ -13249,7 +13261,7 @@
       <c r="AB33" s="34">
         <v>104.25700000000001</v>
       </c>
-      <c r="AC33" s="37">
+      <c r="AC33">
         <v>104.25700000000001</v>
       </c>
       <c r="AD33" s="34">
@@ -13421,7 +13433,7 @@
       <c r="AB34" s="34">
         <v>101.858</v>
       </c>
-      <c r="AC34" s="37">
+      <c r="AC34">
         <v>101.858</v>
       </c>
       <c r="AD34" s="34">
@@ -13593,7 +13605,7 @@
       <c r="AB35" s="34">
         <v>4.343</v>
       </c>
-      <c r="AC35" s="37">
+      <c r="AC35">
         <v>4.343</v>
       </c>
       <c r="AD35" s="34">
@@ -13765,7 +13777,7 @@
       <c r="AB36" s="34">
         <v>20.442</v>
       </c>
-      <c r="AC36" s="37">
+      <c r="AC36">
         <v>20.442</v>
       </c>
       <c r="AD36" s="34">
@@ -13937,7 +13949,7 @@
       <c r="AB37" s="34">
         <v>100.57899999999999</v>
       </c>
-      <c r="AC37" s="37">
+      <c r="AC37">
         <v>100.57899999999999</v>
       </c>
       <c r="AD37" s="34">
@@ -14109,7 +14121,7 @@
       <c r="AB38" s="34">
         <v>41.039000000000001</v>
       </c>
-      <c r="AC38" s="37">
+      <c r="AC38">
         <v>41.039000000000001</v>
       </c>
       <c r="AD38" s="34">
@@ -14281,7 +14293,7 @@
       <c r="AB39" s="34">
         <v>66.700999999999993</v>
       </c>
-      <c r="AC39" s="37">
+      <c r="AC39">
         <v>66.700999999999993</v>
       </c>
       <c r="AD39" s="34">
@@ -14453,7 +14465,7 @@
       <c r="AB40" s="34">
         <v>81.911000000000001</v>
       </c>
-      <c r="AC40" s="37">
+      <c r="AC40">
         <v>81.911000000000001</v>
       </c>
       <c r="AD40" s="34">
@@ -14625,7 +14637,7 @@
       <c r="AB41" s="34">
         <v>23.472000000000001</v>
       </c>
-      <c r="AC41" s="37">
+      <c r="AC41">
         <v>23.472000000000001</v>
       </c>
       <c r="AD41" s="34">
@@ -14797,7 +14809,7 @@
       <c r="AB42" s="34">
         <v>2.6720000000000002</v>
       </c>
-      <c r="AC42" s="37">
+      <c r="AC42">
         <v>2.6720000000000002</v>
       </c>
       <c r="AD42" s="34">
@@ -14969,7 +14981,7 @@
       <c r="AB43" s="34">
         <v>5.319</v>
       </c>
-      <c r="AC43" s="37">
+      <c r="AC43">
         <v>5.319</v>
       </c>
       <c r="AD43" s="34">
@@ -15141,7 +15153,7 @@
       <c r="AB44" s="34">
         <v>39.122999999999998</v>
       </c>
-      <c r="AC44" s="37">
+      <c r="AC44">
         <v>39.122999999999998</v>
       </c>
       <c r="AD44" s="34">
@@ -15313,7 +15325,7 @@
       <c r="AB45" s="34">
         <v>83.960999999999999</v>
       </c>
-      <c r="AC45" s="37">
+      <c r="AC45">
         <v>83.960999999999999</v>
       </c>
       <c r="AD45" s="34">
@@ -15485,7 +15497,7 @@
       <c r="AB46" s="34">
         <v>88.448999999999998</v>
       </c>
-      <c r="AC46" s="37">
+      <c r="AC46">
         <v>88.448999999999998</v>
       </c>
       <c r="AD46" s="34">
@@ -15657,7 +15669,7 @@
       <c r="AB47" s="34">
         <v>34.962000000000003</v>
       </c>
-      <c r="AC47" s="37">
+      <c r="AC47">
         <v>34.962000000000003</v>
       </c>
       <c r="AD47" s="34">
@@ -15829,7 +15841,7 @@
       <c r="AB48" s="34">
         <v>31.841000000000001</v>
       </c>
-      <c r="AC48" s="37">
+      <c r="AC48">
         <v>31.841000000000001</v>
       </c>
       <c r="AD48" s="34">
@@ -16001,7 +16013,7 @@
       <c r="AB49" s="34">
         <v>116.002</v>
       </c>
-      <c r="AC49" s="37">
+      <c r="AC49">
         <v>116.002</v>
       </c>
       <c r="AD49" s="34">
@@ -16173,7 +16185,7 @@
       <c r="AB50" s="34">
         <v>59.149000000000001</v>
       </c>
-      <c r="AC50" s="37">
+      <c r="AC50">
         <v>59.149000000000001</v>
       </c>
       <c r="AD50" s="34">
@@ -16345,7 +16357,7 @@
       <c r="AB51" s="34">
         <v>98.251000000000005</v>
       </c>
-      <c r="AC51" s="37">
+      <c r="AC51">
         <v>98.251000000000005</v>
       </c>
       <c r="AD51" s="34">
@@ -16517,7 +16529,7 @@
       <c r="AB52" s="34">
         <v>84.126999999999995</v>
       </c>
-      <c r="AC52" s="37">
+      <c r="AC52">
         <v>84.126999999999995</v>
       </c>
       <c r="AD52" s="34">
@@ -16679,7 +16691,7 @@
       <c r="AB54" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="AC54" s="38"/>
+      <c r="AC54" s="37"/>
       <c r="AD54" s="33" t="s">
         <v>160</v>
       </c>
@@ -16827,7 +16839,7 @@
       <c r="AB55" s="34">
         <v>31.949000000000002</v>
       </c>
-      <c r="AC55" s="37">
+      <c r="AC55">
         <v>31.949000000000002</v>
       </c>
       <c r="AD55" s="34">
@@ -16999,7 +17011,7 @@
       <c r="AB56" s="34">
         <v>26.696000000000002</v>
       </c>
-      <c r="AC56" s="37">
+      <c r="AC56">
         <v>26.696000000000002</v>
       </c>
       <c r="AD56" s="34">
@@ -17171,7 +17183,7 @@
       <c r="AB57" s="34">
         <v>62.587000000000003</v>
       </c>
-      <c r="AC57" s="37">
+      <c r="AC57">
         <v>62.587000000000003</v>
       </c>
       <c r="AD57" s="34">
@@ -17343,7 +17355,7 @@
       <c r="AB58" s="34">
         <v>50.118000000000002</v>
       </c>
-      <c r="AC58" s="37">
+      <c r="AC58">
         <v>50.118000000000002</v>
       </c>
       <c r="AD58" s="34">
@@ -17515,7 +17527,7 @@
       <c r="AB59" s="34">
         <v>111.27500000000001</v>
       </c>
-      <c r="AC59" s="37">
+      <c r="AC59">
         <v>111.27500000000001</v>
       </c>
       <c r="AD59" s="34">
@@ -17687,7 +17699,7 @@
       <c r="AB60" s="34">
         <v>132.506</v>
       </c>
-      <c r="AC60" s="37">
+      <c r="AC60">
         <v>132.506</v>
       </c>
       <c r="AD60" s="34">
@@ -17859,7 +17871,7 @@
       <c r="AB61" s="34">
         <v>63.453000000000003</v>
       </c>
-      <c r="AC61" s="37">
+      <c r="AC61">
         <v>63.453000000000003</v>
       </c>
       <c r="AD61" s="34">
@@ -18031,7 +18043,7 @@
       <c r="AB62" s="34">
         <v>32.465000000000003</v>
       </c>
-      <c r="AC62" s="37">
+      <c r="AC62">
         <v>32.465000000000003</v>
       </c>
       <c r="AD62" s="34">
@@ -18203,7 +18215,7 @@
       <c r="AB63" s="34">
         <v>124.506</v>
       </c>
-      <c r="AC63" s="37">
+      <c r="AC63">
         <v>124.506</v>
       </c>
       <c r="AD63" s="34">
@@ -18375,7 +18387,7 @@
       <c r="AB64" s="34">
         <v>105.483</v>
       </c>
-      <c r="AC64" s="37">
+      <c r="AC64">
         <v>105.483</v>
       </c>
       <c r="AD64" s="34">
@@ -18547,7 +18559,7 @@
       <c r="AB65" s="34">
         <v>111.34699999999999</v>
       </c>
-      <c r="AC65" s="37">
+      <c r="AC65">
         <v>111.34699999999999</v>
       </c>
       <c r="AD65" s="34">
@@ -18719,7 +18731,7 @@
       <c r="AB66" s="34">
         <v>97.671999999999997</v>
       </c>
-      <c r="AC66" s="37">
+      <c r="AC66">
         <v>97.671999999999997</v>
       </c>
       <c r="AD66" s="34">
@@ -18891,7 +18903,7 @@
       <c r="AB67" s="34">
         <v>37.828000000000003</v>
       </c>
-      <c r="AC67" s="37">
+      <c r="AC67">
         <v>37.828000000000003</v>
       </c>
       <c r="AD67" s="34">
@@ -19063,7 +19075,7 @@
       <c r="AB68" s="34">
         <v>35.167000000000002</v>
       </c>
-      <c r="AC68" s="37">
+      <c r="AC68">
         <v>35.167000000000002</v>
       </c>
       <c r="AD68" s="34">
@@ -19235,7 +19247,7 @@
       <c r="AB69" s="34">
         <v>87.031999999999996</v>
       </c>
-      <c r="AC69" s="37">
+      <c r="AC69">
         <v>87.031999999999996</v>
       </c>
       <c r="AD69" s="34">
@@ -19407,7 +19419,7 @@
       <c r="AB70" s="34">
         <v>56.527999999999999</v>
       </c>
-      <c r="AC70" s="37">
+      <c r="AC70">
         <v>56.527999999999999</v>
       </c>
       <c r="AD70" s="34">
@@ -19579,7 +19591,7 @@
       <c r="AB71" s="34">
         <v>103.697</v>
       </c>
-      <c r="AC71" s="37">
+      <c r="AC71">
         <v>103.697</v>
       </c>
       <c r="AD71" s="34">
@@ -19751,7 +19763,7 @@
       <c r="AB72" s="34">
         <v>109.33499999999999</v>
       </c>
-      <c r="AC72" s="37">
+      <c r="AC72">
         <v>109.33499999999999</v>
       </c>
       <c r="AD72" s="34">
@@ -19923,7 +19935,7 @@
       <c r="AB73" s="34">
         <v>31.059000000000001</v>
       </c>
-      <c r="AC73" s="37">
+      <c r="AC73">
         <v>31.059000000000001</v>
       </c>
       <c r="AD73" s="34">
@@ -20095,7 +20107,7 @@
       <c r="AB74" s="34">
         <v>29.152000000000001</v>
       </c>
-      <c r="AC74" s="37">
+      <c r="AC74">
         <v>29.152000000000001</v>
       </c>
       <c r="AD74" s="34">
@@ -20267,7 +20279,7 @@
       <c r="AB75" s="34">
         <v>68.275999999999996</v>
       </c>
-      <c r="AC75" s="37">
+      <c r="AC75">
         <v>68.275999999999996</v>
       </c>
       <c r="AD75" s="34">
@@ -20439,7 +20451,7 @@
       <c r="AB76" s="34">
         <v>49.231000000000002</v>
       </c>
-      <c r="AC76" s="37">
+      <c r="AC76">
         <v>49.231000000000002</v>
       </c>
       <c r="AD76" s="34">
@@ -20611,7 +20623,7 @@
       <c r="AB77" s="34">
         <v>114.916</v>
       </c>
-      <c r="AC77" s="37">
+      <c r="AC77">
         <v>114.916</v>
       </c>
       <c r="AD77" s="34">
@@ -20782,7 +20794,7 @@
       <c r="AB78" s="34">
         <v>119.821</v>
       </c>
-      <c r="AC78" s="37">
+      <c r="AC78">
         <v>119.821</v>
       </c>
       <c r="AD78" s="34">
@@ -20868,23 +20880,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83328B69-DF3F-45D9-ACCE-8AB412196A0F}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B050DBC2-53C3-44C0-AFE4-F1F0F29FBC79}">
+  <dimension ref="B5:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B050DBC2-53C3-44C0-AFE4-F1F0F29FBC79}">
-  <dimension ref="B5:N17"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20893,102 +20893,106 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="25">
+      <c r="E5" s="26">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>1</v>
+      </c>
+      <c r="G5" s="27">
+        <v>2</v>
+      </c>
+      <c r="H5" s="27">
+        <v>2</v>
+      </c>
+      <c r="I5" s="27">
+        <v>2</v>
+      </c>
+      <c r="J5" s="27">
+        <v>2</v>
+      </c>
+      <c r="K5" s="27">
+        <v>2</v>
+      </c>
+      <c r="L5" s="28">
+        <v>3</v>
+      </c>
+      <c r="M5" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="25">
         <v>0</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E6" s="25">
         <v>1</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F6" s="25">
         <v>2</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G6" s="25">
         <v>3</v>
       </c>
-      <c r="H5" s="25">
+      <c r="H6" s="25">
         <v>4</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I6" s="25">
         <v>5</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J6" s="25">
         <v>6</v>
       </c>
-      <c r="K5" s="25">
+      <c r="K6" s="25">
         <v>7</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L6" s="25">
         <v>8</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M6" s="25">
         <v>9</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N6" s="25">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="25">
+    <row r="7" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="25">
         <v>0</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-    </row>
-    <row r="7" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="25">
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="N7" s="29" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="26">
         <v>1</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="25">
-        <v>0</v>
-      </c>
-      <c r="F7" s="25">
-        <v>0</v>
-      </c>
-      <c r="G7" s="25">
-        <v>0</v>
-      </c>
-      <c r="H7" s="25">
-        <v>0</v>
-      </c>
-      <c r="I7" s="25">
-        <v>0</v>
-      </c>
-      <c r="J7" s="25">
-        <v>0</v>
-      </c>
-      <c r="K7" s="25">
-        <v>0</v>
-      </c>
-      <c r="L7" s="25">
-        <v>0</v>
-      </c>
-      <c r="M7" s="25">
-        <v>0</v>
-      </c>
-      <c r="N7" s="29"/>
-    </row>
-    <row r="8" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
       <c r="C8" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="25">
         <v>0</v>
@@ -20999,8 +21003,8 @@
       <c r="I8" s="25">
         <v>0</v>
       </c>
-      <c r="J8" s="25">
-        <v>0</v>
+      <c r="J8" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="K8" s="25">
         <v>0</v>
@@ -21011,19 +21015,23 @@
       <c r="M8" s="25">
         <v>0</v>
       </c>
-      <c r="N8" s="29"/>
+      <c r="N8" s="29" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="9" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
+      <c r="B9" s="26">
+        <v>1</v>
+      </c>
       <c r="C9" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="25">
         <v>0</v>
@@ -21031,8 +21039,8 @@
       <c r="H9" s="25">
         <v>0</v>
       </c>
-      <c r="I9" s="25">
-        <v>0</v>
+      <c r="I9" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="J9" s="25">
         <v>0</v>
@@ -21046,25 +21054,29 @@
       <c r="M9" s="25">
         <v>0</v>
       </c>
-      <c r="N9" s="29"/>
+      <c r="N9" s="29" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="10" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
+      <c r="B10" s="26">
+        <v>1</v>
+      </c>
       <c r="C10" s="25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="25">
         <v>0</v>
       </c>
-      <c r="H10" s="25">
-        <v>0</v>
+      <c r="H10" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="I10" s="25">
         <v>0</v>
@@ -21081,12 +21093,16 @@
       <c r="M10" s="25">
         <v>0</v>
       </c>
-      <c r="N10" s="29"/>
+      <c r="N10" s="29" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="11" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
+      <c r="B11" s="28">
+        <v>3</v>
+      </c>
       <c r="C11" s="25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="25">
@@ -21095,8 +21111,8 @@
       <c r="F11" s="25">
         <v>0</v>
       </c>
-      <c r="G11" s="25">
-        <v>0</v>
+      <c r="G11" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="H11" s="25">
         <v>0</v>
@@ -21111,24 +21127,28 @@
         <v>0</v>
       </c>
       <c r="L11" s="25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M11" s="25">
-        <v>0</v>
-      </c>
-      <c r="N11" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="N11" s="29" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="12" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
+      <c r="B12" s="28">
+        <v>3</v>
+      </c>
       <c r="C12" s="25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="25">
         <v>0</v>
       </c>
-      <c r="F12" s="25">
-        <v>0</v>
+      <c r="F12" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="G12" s="25">
         <v>0</v>
@@ -21146,39 +21166,43 @@
         <v>0</v>
       </c>
       <c r="L12" s="25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M12" s="25">
-        <v>0</v>
-      </c>
-      <c r="N12" s="29"/>
+        <v>3</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="13" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
+      <c r="B13" s="27">
+        <v>2</v>
+      </c>
       <c r="C13" s="25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="25">
         <v>0</v>
       </c>
-      <c r="F13" s="25">
-        <v>0</v>
+      <c r="F13" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="G13" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13" s="25">
         <v>0</v>
@@ -21186,34 +21210,38 @@
       <c r="M13" s="25">
         <v>0</v>
       </c>
-      <c r="N13" s="29"/>
+      <c r="N13" s="29" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="14" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27"/>
+      <c r="B14" s="27">
+        <v>2</v>
+      </c>
       <c r="C14" s="25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="25">
         <v>0</v>
       </c>
-      <c r="F14" s="25">
-        <v>0</v>
+      <c r="F14" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="G14" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H14" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K14" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L14" s="25">
         <v>0</v>
@@ -21221,84 +21249,152 @@
       <c r="M14" s="25">
         <v>0</v>
       </c>
-      <c r="N14" s="29"/>
+      <c r="N14" s="29" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="15" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
+      <c r="B15" s="27">
+        <v>2</v>
+      </c>
       <c r="C15" s="25">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="25">
         <v>0</v>
       </c>
-      <c r="F15" s="25">
-        <v>0</v>
+      <c r="F15" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="G15" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H15" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15" s="25">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" s="25">
         <v>0</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="N15" s="29"/>
+    </row>
+    <row r="16" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="27">
+        <v>2</v>
+      </c>
+      <c r="C16" s="25">
+        <v>9</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="G16" s="25">
+        <v>2</v>
+      </c>
+      <c r="H16" s="25">
+        <v>2</v>
+      </c>
+      <c r="I16" s="25">
+        <v>2</v>
+      </c>
+      <c r="J16" s="25">
+        <v>2</v>
+      </c>
+      <c r="K16" s="25">
+        <v>2</v>
+      </c>
+      <c r="L16" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="M16" s="25">
         <v>0</v>
       </c>
-      <c r="N15" s="29"/>
-    </row>
-    <row r="16" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="25">
+      <c r="N16" s="29"/>
+    </row>
+    <row r="17" spans="3:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="25">
         <v>10</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-    </row>
-    <row r="17" spans="5:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
+      <c r="D17" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+    </row>
+    <row r="18" spans="3:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+    </row>
+    <row r="21" spans="3:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="25">
+        <v>4.5</v>
+      </c>
+      <c r="F22" s="25">
+        <v>5.5</v>
+      </c>
+      <c r="G22" s="25">
+        <v>5.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2773F724-CF7A-4F4D-A6FE-58AF894E9666}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>